<commit_message>
New model with alignment for T0792, ppt and excel update
</commit_message>
<xml_diff>
--- a/ComporativeProteinModelling.xlsx
+++ b/ComporativeProteinModelling.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TM and RMSD" sheetId="1" r:id="rId1"/>
+    <sheet name="MolProbity" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>T0843</t>
   </si>
@@ -61,12 +62,59 @@
   <si>
     <t>Molprobity</t>
   </si>
+  <si>
+    <t>Protein Geometry</t>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ẞ Deviations &gt;0.25 (Goal=0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Bad bonds (Goal=0%)</t>
+  </si>
+  <si>
+    <t>Bad angles (Goal&lt;0.1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ramchandran favored (Goal&gt;98%)</t>
+  </si>
+  <si>
+    <t>Ramachandran outliers  (Goal&lt;0.05%)</t>
+  </si>
+  <si>
+    <t>Favored roatamers  (Goal&gt;98%)</t>
+  </si>
+  <si>
+    <t>Poor rotamers (Goal&lt;0.3%)</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +122,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,8 +188,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,7 +321,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'TM and RMSD'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -215,6 +341,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -273,7 +400,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>'TM and RMSD'!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -302,7 +429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>'TM and RMSD'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -332,7 +459,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-929B-44E8-BEA4-8F6449E70CF8}"/>
+              <c16:uniqueId val="{00000000-16EB-4B8E-BD09-0C9966BF7F42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -341,7 +468,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'TM and RMSD'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -419,7 +546,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>'TM and RMSD'!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -448,7 +575,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>'TM and RMSD'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -461,6 +588,9 @@
                 <c:pt idx="2">
                   <c:v>0.79</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82940000000000003</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>0.76</c:v>
                 </c:pt>
@@ -469,7 +599,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-929B-44E8-BEA4-8F6449E70CF8}"/>
+              <c16:uniqueId val="{00000001-16EB-4B8E-BD09-0C9966BF7F42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -484,11 +614,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="457294256"/>
-        <c:axId val="457294584"/>
+        <c:axId val="316038312"/>
+        <c:axId val="316044544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457294256"/>
+        <c:axId val="316038312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457294584"/>
+        <c:crossAx val="316044544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457294584"/>
+        <c:axId val="316044544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,10 +693,48 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457294256"/>
+        <c:crossAx val="316038312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1211,23 +1379,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12EA473-4B86-4BBD-9550-BC7BF99B394C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{643C05E4-5DE6-45C8-B79D-07D21C08902C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1547,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="A10:C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,6 +1808,9 @@
       <c r="B5">
         <v>0.9627</v>
       </c>
+      <c r="C5">
+        <v>0.82940000000000003</v>
+      </c>
       <c r="G5" t="s">
         <v>3</v>
       </c>
@@ -1793,4 +1964,455 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="A3:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.23E-2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.9556</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.96309999999999996</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.93869999999999998</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.93149999999999999</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.93340000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.96460000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.98370000000000002</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.96809999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.34E-2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.72E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.49E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.32E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.96460000000000001</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1.34E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="F15" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.9556</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.96309999999999996</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.98370000000000002</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>9.4000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.23E-2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.93869999999999998</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.93149999999999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1.49E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.93340000000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1.32E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some results and PPT final Update
</commit_message>
<xml_diff>
--- a/ComporativeProteinModelling.xlsx
+++ b/ComporativeProteinModelling.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ComparativeProteinModelling\Comparative-Protein-Modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="TM and RMSD" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>T0843</t>
   </si>
@@ -98,6 +98,9 @@
     <t>Poor rotamers (Goal&lt;0.3%)</t>
   </si>
   <si>
+    <t>T0651</t>
+  </si>
+  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -108,13 +111,19 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>cẞ Deviations &gt;0.25 (Goal=0)</t>
+  </si>
+  <si>
+    <t>1, 1.27, 1.11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +146,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +208,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,11 +229,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,8 +278,42 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -255,31 +344,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>TM-Score</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -293,13 +357,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -331,78 +401,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TM and RMSD'!$A$2:$A$8</c:f>
+              <c:f>'TM and RMSD'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>T0843</c:v>
                 </c:pt>
@@ -423,16 +464,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>T0694</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T0651</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TM and RMSD'!$B$2:$B$8</c:f>
+              <c:f>'TM and RMSD'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.88660000000000005</c:v>
                 </c:pt>
@@ -453,13 +497,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.95760000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-16EB-4B8E-BD09-0C9966BF7F42}"/>
+              <c16:uniqueId val="{00000000-16AE-4074-BA85-FB5043C95634}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -478,77 +525,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TM and RMSD'!$A$2:$A$8</c:f>
+              <c:f>'TM and RMSD'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>T0843</c:v>
                 </c:pt>
@@ -569,16 +588,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>T0694</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T0651</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TM and RMSD'!$C$2:$C$8</c:f>
+              <c:f>'TM and RMSD'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.94</c:v>
                 </c:pt>
@@ -599,38 +621,87 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-16EB-4B8E-BD09-0C9966BF7F42}"/>
+              <c16:uniqueId val="{00000001-16AE-4074-BA85-FB5043C95634}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="444"/>
-        <c:overlap val="-90"/>
-        <c:axId val="316038312"/>
-        <c:axId val="316044544"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="442717776"/>
+        <c:axId val="441970920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316038312"/>
+        <c:axId val="442717776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441970920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441970920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -644,14 +715,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -660,11 +725,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -675,66 +739,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316044544"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="316044544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="316038312"/>
+        <c:crossAx val="442717776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -744,7 +752,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -760,9 +768,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -779,17 +786,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -852,79 +870,81 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -940,14 +960,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -956,45 +968,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1006,17 +1008,14 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1025,15 +1024,15 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1049,17 +1048,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1071,7 +1069,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1082,9 +1080,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1095,16 +1093,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1113,14 +1112,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1132,7 +1130,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1140,14 +1138,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1159,14 +1157,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1177,16 +1175,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1195,14 +1194,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1213,27 +1212,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1241,17 +1239,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1264,14 +1261,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1283,12 +1280,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1297,14 +1301,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1313,19 +1316,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1333,9 +1335,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1346,22 +1348,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1369,7 +1359,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1379,23 +1369,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{643C05E4-5DE6-45C8-B79D-07D21C08902C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884846DD-A99C-43B1-964C-69CF1CAC800F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,6 +1865,20 @@
         <v>0.224</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0.9788</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>0.249</v>
+      </c>
+    </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
@@ -1958,6 +1962,17 @@
       </c>
       <c r="C17">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1968,25 +1983,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H20"/>
+  <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="A3:H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1995,215 +2010,240 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:9" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="I3" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="12">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="13">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
         <v>1.23E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="12">
         <v>4.1099999999999998E-2</v>
       </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1.7399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="15">
         <v>0.93669999999999998</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="15">
         <v>0.92200000000000004</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="13">
         <v>0.9556</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="13">
         <v>0.96309999999999996</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="15">
         <v>0.93869999999999998</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="15">
         <v>0.93149999999999999</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="15">
         <v>0.93340000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="I5" s="12">
+        <v>0.92610000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="15">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="12">
         <v>3.1699999999999999E-2</v>
       </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
         <v>3.2000000000000002E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="I6" s="12">
+        <v>7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="13">
         <v>0.96460000000000001</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="15">
         <v>0.92059999999999997</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="16">
         <v>0.97660000000000002</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="17">
         <v>0.98370000000000002</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="18">
         <v>0.90669999999999995</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="16">
         <v>0.97440000000000004</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="13">
         <v>0.96809999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="I7" s="19">
+        <v>98.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="12">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="C9" s="11">
-        <v>0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="12">
         <v>1.34E-2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="12">
         <v>1.72E-2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="12">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="12">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="12">
         <v>1.49E-2</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="12">
         <v>1.32E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2229,7 +2269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2295,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
@@ -2281,7 +2321,7 @@
         <v>1.72E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>